<commit_message>
update print excel tpp report
</commit_message>
<xml_diff>
--- a/hello world.xlsx
+++ b/hello world.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
   <si>
     <t>PERHITUNGAN TAMBAHAN PENGHASILAN KECAMATAN SETU KABUPATEN BEKASI</t>
   </si>
@@ -65,6 +65,24 @@
     <t>PRODUKTIVITAS KERJA</t>
   </si>
   <si>
+    <t>60%</t>
+  </si>
+  <si>
+    <t>TAMBAHAN TPP</t>
+  </si>
+  <si>
+    <t>Pj / Plt / JABATAN FUNGSIONAL BUKAN PENYETARAAN DENGAN TUGAS TAMBAHAN SEBAGAI KOORDINATOR / SUBKOORDINATOR</t>
+  </si>
+  <si>
+    <t>PENGURANGAN TPP</t>
+  </si>
+  <si>
+    <t>KELEBIHAN BAYAR DESEMBER / TERJARING GERAKAN DISIPLIN APARATUR /MANIPULASI DATA / LHKPN / LHKASN</t>
+  </si>
+  <si>
+    <t>JUMLAH TPP DITERIMA</t>
+  </si>
+  <si>
     <t>Drs. JOKO DWOJATMOKO, M.Si</t>
   </si>
   <si>
@@ -72,6 +90,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>100 %</t>
   </si>
 </sst>
 </file>
@@ -79,7 +100,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -104,6 +125,15 @@
       <strike val="0"/>
       <u val="none"/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Bookman Old Style"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="7"/>
       <color rgb="FF000000"/>
       <name val="Bookman Old Style"/>
     </font>
@@ -174,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -204,6 +234,9 @@
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
@@ -513,10 +546,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:U8"/>
+  <dimension ref="A1:W8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="D7" sqref="D7:H7"/>
+      <selection activeCell="D7" sqref="D7:W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -542,9 +575,11 @@
     <col min="19" max="19" width="18" customWidth="true" style="0"/>
     <col min="20" max="20" width="18" customWidth="true" style="0"/>
     <col min="21" max="21" width="18" customWidth="true" style="0"/>
+    <col min="22" max="22" width="18" customWidth="true" style="0"/>
+    <col min="23" max="23" width="18" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:23">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -568,8 +603,10 @@
       <c r="S1" s="9"/>
       <c r="T1" s="9"/>
       <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:23">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -593,8 +630,10 @@
       <c r="S2" s="9"/>
       <c r="T2" s="9"/>
       <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:23" customHeight="1" ht="30">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -627,9 +666,17 @@
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
+      <c r="U3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:23" customHeight="1" ht="30">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -652,15 +699,21 @@
         <v>13</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
+      <c r="U4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="V4" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="W4" s="4"/>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:23" customHeight="1" ht="30">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -695,25 +748,27 @@
       <c r="N5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="O5" s="5" t="s">
+      <c r="O5" s="4"/>
+      <c r="P5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="P5" s="6" t="s">
+      <c r="Q5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="Q5" s="7" t="s">
+      <c r="R5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="R5" s="8" t="s">
+      <c r="S5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="S5" s="4" t="s">
+      <c r="T5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="T5" s="4"/>
-      <c r="U5" s="4"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="4"/>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:23">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -777,47 +832,85 @@
       <c r="U6" s="1">
         <v>21</v>
       </c>
+      <c r="V6" s="1">
+        <v>22</v>
+      </c>
+      <c r="W6" s="1">
+        <v>23</v>
+      </c>
     </row>
-    <row r="7" spans="1:21">
-      <c r="A7" s="10">
+    <row r="7" spans="1:23">
+      <c r="A7" s="11">
         <v>1</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="12">
+      <c r="B7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="13">
         <v>11340000</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="13">
         <v>14580000</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="13">
         <v>6480000</v>
       </c>
-      <c r="G7" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="12">
+      <c r="G7" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="13">
         <v>32400000</v>
       </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
+      <c r="I7" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="13">
+        <v>4536000</v>
+      </c>
+      <c r="K7" s="13">
+        <v>5832000</v>
+      </c>
+      <c r="L7" s="13">
+        <v>2592000</v>
+      </c>
+      <c r="M7" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="N7" s="13">
+        <v>12960000</v>
+      </c>
+      <c r="O7" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="P7" s="13">
+        <v>6804000</v>
+      </c>
+      <c r="Q7" s="13">
+        <v>8748000</v>
+      </c>
+      <c r="R7" s="13">
+        <v>3888000</v>
+      </c>
+      <c r="S7" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="T7" s="13">
+        <v>19440000</v>
+      </c>
+      <c r="U7" s="13">
+        <v>0</v>
+      </c>
+      <c r="V7" s="13">
+        <v>0</v>
+      </c>
+      <c r="W7" s="13">
+        <v>64800000</v>
+      </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:23">
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -836,12 +929,14 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A1:W1"/>
+    <mergeCell ref="A2:W2"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:C5"/>
@@ -850,9 +945,12 @@
     <mergeCell ref="I3:N3"/>
     <mergeCell ref="J4:N4"/>
     <mergeCell ref="I4:I5"/>
-    <mergeCell ref="O3:U3"/>
-    <mergeCell ref="P4:U4"/>
+    <mergeCell ref="O3:T3"/>
+    <mergeCell ref="P4:T4"/>
     <mergeCell ref="O4:O5"/>
+    <mergeCell ref="U4:U5"/>
+    <mergeCell ref="V4:V5"/>
+    <mergeCell ref="W3:W5"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
udpate hitungan tpp & capaian kinerja. Update tipe data untuk kolom nilai menggunakan decimal
</commit_message>
<xml_diff>
--- a/hello world.xlsx
+++ b/hello world.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
   <si>
     <t>PERHITUNGAN TAMBAHAN PENGHASILAN KECAMATAN SETU KABUPATEN BEKASI</t>
   </si>
@@ -92,7 +92,19 @@
     <t>-</t>
   </si>
   <si>
-    <t>100 %</t>
+    <t>100.00 %</t>
+  </si>
+  <si>
+    <t>IRVAN HERMAWAN, A.Md</t>
+  </si>
+  <si>
+    <t>PENGELOLA PEMBERDAYAAN MASYARAKAT DAN KELEMBAGAAN</t>
+  </si>
+  <si>
+    <t>76.00 %</t>
+  </si>
+  <si>
+    <t>54.55 %</t>
   </si>
 </sst>
 </file>
@@ -546,10 +558,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:W8"/>
+  <dimension ref="A1:W9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="D7" sqref="D7:W7"/>
+      <selection activeCell="D7" sqref="D7:W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -862,7 +874,7 @@
         <v>24</v>
       </c>
       <c r="H7" s="13">
-        <v>32400000</v>
+        <v>32400000.0</v>
       </c>
       <c r="I7" s="13" t="s">
         <v>25</v>
@@ -901,36 +913,107 @@
         <v>19440000</v>
       </c>
       <c r="U7" s="13">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="V7" s="13">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="W7" s="13">
-        <v>64800000</v>
+        <v>32400000.0</v>
       </c>
     </row>
     <row r="8" spans="1:23">
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
+      <c r="A8" s="11">
+        <v>2</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="13">
+        <v>2065000</v>
+      </c>
+      <c r="E8" s="13">
+        <v>2655000</v>
+      </c>
+      <c r="F8" s="13">
+        <v>1180000</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="13">
+        <v>5900000.0</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="13">
+        <v>627760</v>
+      </c>
+      <c r="K8" s="13">
+        <v>807120</v>
+      </c>
+      <c r="L8" s="13">
+        <v>358720</v>
+      </c>
+      <c r="M8" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="N8" s="13">
+        <v>1793600</v>
+      </c>
+      <c r="O8" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="P8" s="13">
+        <v>675875</v>
+      </c>
+      <c r="Q8" s="13">
+        <v>868982</v>
+      </c>
+      <c r="R8" s="13">
+        <v>386214</v>
+      </c>
+      <c r="S8" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="T8" s="13">
+        <v>1931070</v>
+      </c>
+      <c r="U8" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="V8" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="W8" s="13">
+        <v>3724670.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
update besaran tpp hapus penambahan tpp, dan udpate excel print tpp:
</commit_message>
<xml_diff>
--- a/hello world.xlsx
+++ b/hello world.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
   <si>
     <t>PERHITUNGAN TAMBAHAN PENGHASILAN KECAMATAN SETU KABUPATEN BEKASI</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>54.55 %</t>
+  </si>
+  <si>
+    <t>JUMLAH</t>
   </si>
 </sst>
 </file>
@@ -223,9 +226,6 @@
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="4" fillId="0" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -258,6 +258,9 @@
     </xf>
     <xf xfId="0" fontId="2" numFmtId="4" fillId="0" borderId="2" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -561,7 +564,7 @@
   <dimension ref="A1:W9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="D7" sqref="D7:W8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -592,193 +595,193 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
     </row>
     <row r="2" spans="1:23">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
     </row>
     <row r="3" spans="1:23" customHeight="1" ht="30">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4" t="s">
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4" t="s">
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4" t="s">
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="V3" s="4" t="s">
+      <c r="V3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="W3" s="4" t="s">
+      <c r="W3" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:23" customHeight="1" ht="30">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4" t="s">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4" t="s">
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="P4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="10" t="s">
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="V4" s="10" t="s">
+      <c r="V4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="W4" s="4"/>
+      <c r="W4" s="3"/>
     </row>
     <row r="5" spans="1:23" customHeight="1" ht="30">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="5" t="s">
+      <c r="I5" s="3"/>
+      <c r="J5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="K5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="M5" s="8" t="s">
+      <c r="M5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="N5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O5" s="4"/>
-      <c r="P5" s="5" t="s">
+      <c r="O5" s="3"/>
+      <c r="P5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="Q5" s="6" t="s">
+      <c r="Q5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="R5" s="7" t="s">
+      <c r="R5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="S5" s="8" t="s">
+      <c r="S5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="T5" s="4" t="s">
+      <c r="T5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="U5" s="10"/>
-      <c r="V5" s="10"/>
-      <c r="W5" s="4"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="3"/>
     </row>
     <row r="6" spans="1:23">
       <c r="A6" s="1">
@@ -852,168 +855,209 @@
       </c>
     </row>
     <row r="7" spans="1:23">
-      <c r="A7" s="11">
+      <c r="A7" s="10">
         <v>1</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="12">
         <v>11340000</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="12">
         <v>14580000</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="12">
         <v>6480000</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="12">
         <v>32400000.0</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="12">
         <v>4536000</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="12">
         <v>5832000</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7" s="12">
         <v>2592000</v>
       </c>
-      <c r="M7" s="13" t="s">
+      <c r="M7" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="N7" s="13">
+      <c r="N7" s="12">
         <v>12960000</v>
       </c>
-      <c r="O7" s="13" t="s">
+      <c r="O7" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="P7" s="13">
+      <c r="P7" s="12">
         <v>6804000</v>
       </c>
-      <c r="Q7" s="13">
+      <c r="Q7" s="12">
         <v>8748000</v>
       </c>
-      <c r="R7" s="13">
+      <c r="R7" s="12">
         <v>3888000</v>
       </c>
-      <c r="S7" s="13" t="s">
+      <c r="S7" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="T7" s="13">
+      <c r="T7" s="12">
         <v>19440000</v>
       </c>
-      <c r="U7" s="13">
+      <c r="U7" s="12">
         <v>0.0</v>
       </c>
-      <c r="V7" s="13">
+      <c r="V7" s="12">
         <v>0.0</v>
       </c>
-      <c r="W7" s="13">
+      <c r="W7" s="12">
         <v>32400000.0</v>
       </c>
     </row>
     <row r="8" spans="1:23">
-      <c r="A8" s="11">
+      <c r="A8" s="10">
         <v>2</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="12">
         <v>2065000</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="12">
         <v>2655000</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="12">
         <v>1180000</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="12">
         <v>5900000.0</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="12">
         <v>627760</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K8" s="12">
         <v>807120</v>
       </c>
-      <c r="L8" s="13">
+      <c r="L8" s="12">
         <v>358720</v>
       </c>
-      <c r="M8" s="13" t="s">
+      <c r="M8" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="N8" s="13">
+      <c r="N8" s="12">
         <v>1793600</v>
       </c>
-      <c r="O8" s="13" t="s">
+      <c r="O8" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="P8" s="13">
+      <c r="P8" s="12">
         <v>675875</v>
       </c>
-      <c r="Q8" s="13">
+      <c r="Q8" s="12">
         <v>868982</v>
       </c>
-      <c r="R8" s="13">
+      <c r="R8" s="12">
         <v>386214</v>
       </c>
-      <c r="S8" s="13" t="s">
+      <c r="S8" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="T8" s="13">
+      <c r="T8" s="12">
         <v>1931070</v>
       </c>
-      <c r="U8" s="13">
+      <c r="U8" s="12">
         <v>0.0</v>
       </c>
-      <c r="V8" s="13">
+      <c r="V8" s="12">
         <v>0.0</v>
       </c>
-      <c r="W8" s="13">
+      <c r="W8" s="12">
         <v>3724670.0</v>
       </c>
     </row>
     <row r="9" spans="1:23">
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2"/>
+      <c r="A9" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="12">
+        <v>13405000</v>
+      </c>
+      <c r="E9" s="12">
+        <v>17235000</v>
+      </c>
+      <c r="F9" s="12">
+        <v>7660000</v>
+      </c>
+      <c r="G9" s="12">
+        <v>0</v>
+      </c>
+      <c r="H9" s="12">
+        <v>38300000.0</v>
+      </c>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12">
+        <v>5163760</v>
+      </c>
+      <c r="K9" s="12">
+        <v>6639120</v>
+      </c>
+      <c r="L9" s="12">
+        <v>2950720</v>
+      </c>
+      <c r="M9" s="12">
+        <v>0</v>
+      </c>
+      <c r="N9" s="12">
+        <v>14753600</v>
+      </c>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12">
+        <v>7479875</v>
+      </c>
+      <c r="Q9" s="12">
+        <v>9616982</v>
+      </c>
+      <c r="R9" s="12">
+        <v>4274214</v>
+      </c>
+      <c r="S9" s="12">
+        <v>0</v>
+      </c>
+      <c r="T9" s="12">
+        <v>21371070</v>
+      </c>
+      <c r="U9" s="12">
+        <v>0</v>
+      </c>
+      <c r="V9" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="W9" s="12">
+        <v>36124670.0</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
@@ -1034,6 +1078,7 @@
     <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="W3:W5"/>
+    <mergeCell ref="A9:C9"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>